<commit_message>
:zap: cmd/output; template can use color
</commit_message>
<xml_diff>
--- a/resource/template.xlsx
+++ b/resource/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mio256/wplus-server/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82490655-C17F-384A-9490-A1370F8D854C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{03A8A258-0119-4A44-8F42-45ECBDEA9CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -235,7 +236,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -415,17 +416,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -573,7 +563,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -616,9 +606,6 @@
     <xf numFmtId="176" fontId="10" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -631,7 +618,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -640,19 +627,19 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
@@ -664,16 +651,16 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -685,7 +672,14 @@
     <cellStyle name="標準 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="標準 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="55">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -747,14 +741,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="4" tint="0.79998168889431442"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -764,7 +753,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -795,6 +784,397 @@
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1141,7 +1521,7 @@
   <dimension ref="B2:AJ18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -1155,15 +1535,15 @@
   <sheetData>
     <row r="2" spans="2:36" ht="31">
       <c r="B2" s="1"/>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
       <c r="J2" s="5"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -1231,9 +1611,7 @@
     </row>
     <row r="4" spans="2:36" ht="21" thickBot="1">
       <c r="B4" s="1"/>
-      <c r="C4" s="7">
-        <v>2024</v>
-      </c>
+      <c r="C4" s="7"/>
       <c r="D4" s="8" t="s">
         <v>7</v>
       </c>
@@ -1268,324 +1646,324 @@
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
-      <c r="AH4" s="26" t="s">
+      <c r="AH4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="AI4" s="27"/>
+      <c r="AI4" s="26"/>
       <c r="AJ4" s="1"/>
     </row>
     <row r="5" spans="2:36" ht="21" thickBot="1">
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="10" t="e">
         <f>DATE($C$4,$E$4,1)</f>
-        <v>45261</v>
-      </c>
-      <c r="D5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="D5" s="10" t="e">
         <f>C5+1</f>
-        <v>45262</v>
-      </c>
-      <c r="E5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="E5" s="10" t="e">
         <f t="shared" ref="E5:AF5" si="0">D5+1</f>
-        <v>45263</v>
-      </c>
-      <c r="F5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="F5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45264</v>
-      </c>
-      <c r="G5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="G5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45265</v>
-      </c>
-      <c r="H5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="H5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45266</v>
-      </c>
-      <c r="I5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="I5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45267</v>
-      </c>
-      <c r="J5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="J5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45268</v>
-      </c>
-      <c r="K5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="K5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45269</v>
-      </c>
-      <c r="L5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="L5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45270</v>
-      </c>
-      <c r="M5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="M5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45271</v>
-      </c>
-      <c r="N5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="N5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45272</v>
-      </c>
-      <c r="O5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="O5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45273</v>
-      </c>
-      <c r="P5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="P5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45274</v>
-      </c>
-      <c r="Q5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45275</v>
-      </c>
-      <c r="R5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="R5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45276</v>
-      </c>
-      <c r="S5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="S5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45277</v>
-      </c>
-      <c r="T5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="T5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45278</v>
-      </c>
-      <c r="U5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="U5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45279</v>
-      </c>
-      <c r="V5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="V5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45280</v>
-      </c>
-      <c r="W5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="W5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45281</v>
-      </c>
-      <c r="X5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="X5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45282</v>
-      </c>
-      <c r="Y5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="Y5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45283</v>
-      </c>
-      <c r="Z5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="Z5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45284</v>
-      </c>
-      <c r="AA5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="AA5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45285</v>
-      </c>
-      <c r="AB5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="AB5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45286</v>
-      </c>
-      <c r="AC5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="AC5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45287</v>
-      </c>
-      <c r="AD5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="AD5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45288</v>
-      </c>
-      <c r="AE5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="AE5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45289</v>
-      </c>
-      <c r="AF5" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="AF5" s="10" t="e">
         <f t="shared" si="0"/>
-        <v>45290</v>
-      </c>
-      <c r="AG5" s="13">
+        <v>#NUM!</v>
+      </c>
+      <c r="AG5" s="13" t="e">
         <f>AF5+1</f>
-        <v>45291</v>
-      </c>
-      <c r="AH5" s="30" t="s">
+        <v>#NUM!</v>
+      </c>
+      <c r="AH5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="AI5" s="32" t="s">
+      <c r="AI5" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="AJ5" s="17" t="s">
+      <c r="AJ5" s="16" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:36" ht="21" thickBot="1">
-      <c r="B6" s="29"/>
-      <c r="C6" s="12">
-        <f>C5</f>
-        <v>45261</v>
-      </c>
-      <c r="D6" s="12">
-        <f t="shared" ref="D6:AG6" si="1">D5</f>
-        <v>45262</v>
-      </c>
-      <c r="E6" s="12">
+      <c r="B6" s="28"/>
+      <c r="C6" s="12" t="e">
+        <f>TEXT(C5,"aaa")</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D6" s="12" t="e">
+        <f t="shared" ref="D6:AG6" si="1">TEXT(D5,"aaa")</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45263</v>
-      </c>
-      <c r="F6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="F6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45264</v>
-      </c>
-      <c r="G6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="G6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45265</v>
-      </c>
-      <c r="H6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="H6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45266</v>
-      </c>
-      <c r="I6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="I6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45267</v>
-      </c>
-      <c r="J6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="J6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45268</v>
-      </c>
-      <c r="K6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="K6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45269</v>
-      </c>
-      <c r="L6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="L6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45270</v>
-      </c>
-      <c r="M6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="M6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45271</v>
-      </c>
-      <c r="N6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="N6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45272</v>
-      </c>
-      <c r="O6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="O6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45273</v>
-      </c>
-      <c r="P6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="P6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45274</v>
-      </c>
-      <c r="Q6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45275</v>
-      </c>
-      <c r="R6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="R6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45276</v>
-      </c>
-      <c r="S6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="S6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45277</v>
-      </c>
-      <c r="T6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="T6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45278</v>
-      </c>
-      <c r="U6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="U6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45279</v>
-      </c>
-      <c r="V6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="V6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45280</v>
-      </c>
-      <c r="W6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="W6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45281</v>
-      </c>
-      <c r="X6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="X6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45282</v>
-      </c>
-      <c r="Y6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="Y6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45283</v>
-      </c>
-      <c r="Z6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="Z6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45284</v>
-      </c>
-      <c r="AA6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="AA6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45285</v>
-      </c>
-      <c r="AB6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="AB6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45286</v>
-      </c>
-      <c r="AC6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="AC6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45287</v>
-      </c>
-      <c r="AD6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="AD6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45288</v>
-      </c>
-      <c r="AE6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="AE6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45289</v>
-      </c>
-      <c r="AF6" s="12">
+        <v>#NUM!</v>
+      </c>
+      <c r="AF6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45290</v>
-      </c>
-      <c r="AG6" s="14">
+        <v>#NUM!</v>
+      </c>
+      <c r="AG6" s="12" t="e">
         <f t="shared" si="1"/>
-        <v>45291</v>
-      </c>
-      <c r="AH6" s="31"/>
-      <c r="AI6" s="33"/>
-      <c r="AJ6" s="18" t="s">
+        <v>#NUM!</v>
+      </c>
+      <c r="AH6" s="30"/>
+      <c r="AI6" s="32"/>
+      <c r="AJ6" s="17" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:36">
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="21"/>
-      <c r="T7" s="21"/>
-      <c r="U7" s="21"/>
-      <c r="V7" s="21"/>
-      <c r="W7" s="21"/>
-      <c r="X7" s="21"/>
-      <c r="Y7" s="21"/>
-      <c r="Z7" s="21"/>
-      <c r="AA7" s="21"/>
-      <c r="AB7" s="21"/>
-      <c r="AC7" s="21"/>
-      <c r="AD7" s="21"/>
-      <c r="AE7" s="21"/>
-      <c r="AF7" s="21"/>
-      <c r="AG7" s="22"/>
-      <c r="AH7" s="23">
-        <f t="shared" ref="AH7:AH8" si="2">SUM(C7:AG7)</f>
-        <v>0</v>
-      </c>
-      <c r="AI7" s="24">
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="20"/>
+      <c r="V7" s="20"/>
+      <c r="W7" s="20"/>
+      <c r="X7" s="20"/>
+      <c r="Y7" s="20"/>
+      <c r="Z7" s="20"/>
+      <c r="AA7" s="20"/>
+      <c r="AB7" s="20"/>
+      <c r="AC7" s="20"/>
+      <c r="AD7" s="20"/>
+      <c r="AE7" s="20"/>
+      <c r="AF7" s="20"/>
+      <c r="AG7" s="21"/>
+      <c r="AH7" s="22">
+        <f>SUM(C7:AG7)</f>
+        <v>0</v>
+      </c>
+      <c r="AI7" s="23">
         <f>COUNT(C7:AG7)</f>
         <v>0</v>
       </c>
-      <c r="AJ7" s="25">
+      <c r="AJ7" s="24">
         <f>AH8</f>
         <v>0</v>
       </c>
@@ -1625,64 +2003,64 @@
       <c r="AE8" s="11"/>
       <c r="AF8" s="11"/>
       <c r="AG8" s="11" t="str">
-        <f t="shared" ref="D8:AG8" si="3">IF(AG7-8&gt;0,AG7-8," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="AH8" s="15">
-        <f t="shared" si="2"/>
+        <f>IF(AG7-8&gt;0,AG7-8," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="AH8" s="14">
+        <f>SUM(C8:AG8)</f>
         <v>0</v>
       </c>
       <c r="AI8" s="4">
         <f>COUNT(C8:AG8)</f>
         <v>0</v>
       </c>
-      <c r="AJ8" s="16">
+      <c r="AJ8" s="15">
         <f>AH7+AH8</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:36">
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="21"/>
-      <c r="X9" s="21"/>
-      <c r="Y9" s="21"/>
-      <c r="Z9" s="21"/>
-      <c r="AA9" s="21"/>
-      <c r="AB9" s="21"/>
-      <c r="AC9" s="21"/>
-      <c r="AD9" s="21"/>
-      <c r="AE9" s="21"/>
-      <c r="AF9" s="21"/>
-      <c r="AG9" s="22"/>
-      <c r="AH9" s="23">
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20"/>
+      <c r="U9" s="20"/>
+      <c r="V9" s="20"/>
+      <c r="W9" s="20"/>
+      <c r="X9" s="20"/>
+      <c r="Y9" s="20"/>
+      <c r="Z9" s="20"/>
+      <c r="AA9" s="20"/>
+      <c r="AB9" s="20"/>
+      <c r="AC9" s="20"/>
+      <c r="AD9" s="20"/>
+      <c r="AE9" s="20"/>
+      <c r="AF9" s="20"/>
+      <c r="AG9" s="21"/>
+      <c r="AH9" s="22">
         <f>SUM(C9:AG9)</f>
         <v>0</v>
       </c>
-      <c r="AI9" s="24">
+      <c r="AI9" s="23">
         <f>COUNT(C9:AG9)</f>
         <v>0</v>
       </c>
-      <c r="AJ9" s="25">
+      <c r="AJ9" s="24">
         <f>AH10</f>
         <v>0</v>
       </c>
@@ -1722,64 +2100,64 @@
       <c r="AE10" s="11"/>
       <c r="AF10" s="11"/>
       <c r="AG10" s="11" t="str">
-        <f t="shared" ref="D10:AG10" si="4">IF(AG9-8&gt;0,AG9-8," ")</f>
-        <v/>
-      </c>
-      <c r="AH10" s="15">
-        <f t="shared" ref="AH9:AH18" si="5">SUM(C10:AG10)</f>
+        <f>IF(AG9-8&gt;0,AG9-8," ")</f>
+        <v/>
+      </c>
+      <c r="AH10" s="14">
+        <f t="shared" ref="AH10:AH18" si="2">SUM(C10:AG10)</f>
         <v>0</v>
       </c>
       <c r="AI10" s="4">
-        <f t="shared" ref="AI9:AI18" si="6">COUNT(C10:AG10)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ10" s="16">
+        <f t="shared" ref="AI10:AI18" si="3">COUNT(C10:AG10)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="15">
         <f>AH9+AH10</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:36">
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="21"/>
-      <c r="S11" s="21"/>
-      <c r="T11" s="21"/>
-      <c r="U11" s="21"/>
-      <c r="V11" s="21"/>
-      <c r="W11" s="21"/>
-      <c r="X11" s="21"/>
-      <c r="Y11" s="21"/>
-      <c r="Z11" s="21"/>
-      <c r="AA11" s="21"/>
-      <c r="AB11" s="21"/>
-      <c r="AC11" s="21"/>
-      <c r="AD11" s="21"/>
-      <c r="AE11" s="21"/>
-      <c r="AF11" s="21"/>
-      <c r="AG11" s="22"/>
-      <c r="AH11" s="23">
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="20"/>
+      <c r="U11" s="20"/>
+      <c r="V11" s="20"/>
+      <c r="W11" s="20"/>
+      <c r="X11" s="20"/>
+      <c r="Y11" s="20"/>
+      <c r="Z11" s="20"/>
+      <c r="AA11" s="20"/>
+      <c r="AB11" s="20"/>
+      <c r="AC11" s="20"/>
+      <c r="AD11" s="20"/>
+      <c r="AE11" s="20"/>
+      <c r="AF11" s="20"/>
+      <c r="AG11" s="21"/>
+      <c r="AH11" s="22">
         <f>SUM(C11:AG11)</f>
         <v>0</v>
       </c>
-      <c r="AI11" s="24">
+      <c r="AI11" s="23">
         <f>COUNT(C11:AG11)</f>
         <v>0</v>
       </c>
-      <c r="AJ11" s="25">
+      <c r="AJ11" s="24">
         <f>AH12</f>
         <v>0</v>
       </c>
@@ -1793,180 +2171,180 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D12" s="11" t="str">
-        <f t="shared" ref="D12:AG12" si="7">IF(D11-8&gt;0,D11-8," ")</f>
+        <f t="shared" ref="D12:AG12" si="4">IF(D11-8&gt;0,D11-8," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="E12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="I12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="J12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="L12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="M12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="N12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="O12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="Q12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="R12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="S12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="T12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="U12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="V12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="W12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="X12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="Y12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="Z12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="AA12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="AB12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="AC12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="AD12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="AE12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="AF12" s="11" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="AG12" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="AH12" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AH12" s="14">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI12" s="4">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AJ12" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="15">
         <f>AH11+AH12</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:36">
-      <c r="B13" s="19"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="21"/>
-      <c r="S13" s="21"/>
-      <c r="T13" s="21"/>
-      <c r="U13" s="21"/>
-      <c r="V13" s="21"/>
-      <c r="W13" s="21"/>
-      <c r="X13" s="21"/>
-      <c r="Y13" s="21"/>
-      <c r="Z13" s="21"/>
-      <c r="AA13" s="21"/>
-      <c r="AB13" s="21"/>
-      <c r="AC13" s="21"/>
-      <c r="AD13" s="21"/>
-      <c r="AE13" s="21"/>
-      <c r="AF13" s="21"/>
-      <c r="AG13" s="22"/>
-      <c r="AH13" s="23">
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="20"/>
+      <c r="T13" s="20"/>
+      <c r="U13" s="20"/>
+      <c r="V13" s="20"/>
+      <c r="W13" s="20"/>
+      <c r="X13" s="20"/>
+      <c r="Y13" s="20"/>
+      <c r="Z13" s="20"/>
+      <c r="AA13" s="20"/>
+      <c r="AB13" s="20"/>
+      <c r="AC13" s="20"/>
+      <c r="AD13" s="20"/>
+      <c r="AE13" s="20"/>
+      <c r="AF13" s="20"/>
+      <c r="AG13" s="21"/>
+      <c r="AH13" s="22">
         <f>SUM(C13:AG13)</f>
         <v>0</v>
       </c>
-      <c r="AI13" s="24">
+      <c r="AI13" s="23">
         <f>COUNT(C13:AG13)</f>
         <v>0</v>
       </c>
-      <c r="AJ13" s="25">
+      <c r="AJ13" s="24">
         <f>AH14</f>
         <v>0</v>
       </c>
@@ -1980,180 +2358,180 @@
         <v/>
       </c>
       <c r="D14" s="11" t="str">
-        <f t="shared" ref="D14:AG14" si="8">IF(D13-8&gt;0,D13-8," ")</f>
+        <f t="shared" ref="D14:AG14" si="5">IF(D13-8&gt;0,D13-8," ")</f>
         <v/>
       </c>
       <c r="E14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="F14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="H14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="J14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="K14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="L14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="M14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="N14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="O14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="P14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="Q14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="R14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="S14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="T14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="U14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="V14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="W14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="X14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="Y14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="Z14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AA14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AB14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AC14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AD14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AE14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AF14" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AG14" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="AH14" s="15">
         <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AH14" s="14">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI14" s="4">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AJ14" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="15">
         <f>AH13+AH14</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:36">
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="21"/>
-      <c r="S15" s="21"/>
-      <c r="T15" s="21"/>
-      <c r="U15" s="21"/>
-      <c r="V15" s="21"/>
-      <c r="W15" s="21"/>
-      <c r="X15" s="21"/>
-      <c r="Y15" s="21"/>
-      <c r="Z15" s="21"/>
-      <c r="AA15" s="21"/>
-      <c r="AB15" s="21"/>
-      <c r="AC15" s="21"/>
-      <c r="AD15" s="21"/>
-      <c r="AE15" s="21"/>
-      <c r="AF15" s="21"/>
-      <c r="AG15" s="22"/>
-      <c r="AH15" s="23">
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="20"/>
+      <c r="U15" s="20"/>
+      <c r="V15" s="20"/>
+      <c r="W15" s="20"/>
+      <c r="X15" s="20"/>
+      <c r="Y15" s="20"/>
+      <c r="Z15" s="20"/>
+      <c r="AA15" s="20"/>
+      <c r="AB15" s="20"/>
+      <c r="AC15" s="20"/>
+      <c r="AD15" s="20"/>
+      <c r="AE15" s="20"/>
+      <c r="AF15" s="20"/>
+      <c r="AG15" s="21"/>
+      <c r="AH15" s="22">
         <f>SUM(C15:AG15)</f>
         <v>0</v>
       </c>
-      <c r="AI15" s="24">
+      <c r="AI15" s="23">
         <f>COUNT(C15:AG15)</f>
         <v>0</v>
       </c>
-      <c r="AJ15" s="25">
+      <c r="AJ15" s="24">
         <f>AH16</f>
         <v>0</v>
       </c>
@@ -2167,180 +2545,180 @@
         <v/>
       </c>
       <c r="D16" s="11" t="str">
-        <f t="shared" ref="D16:AG16" si="9">IF(D15-8&gt;0,D15-8," ")</f>
+        <f t="shared" ref="D16:AG16" si="6">IF(D15-8&gt;0,D15-8," ")</f>
         <v/>
       </c>
       <c r="E16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="H16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="J16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="K16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="L16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="M16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="N16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="O16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Q16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="R16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="S16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="T16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="U16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="V16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="W16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="X16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Z16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AA16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AB16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AC16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AD16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AE16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AF16" s="11" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AG16" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AH16" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AH16" s="14">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI16" s="4">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AJ16" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="15">
         <f>AH15+AH16</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:36">
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="21"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="21"/>
-      <c r="Q17" s="21"/>
-      <c r="R17" s="21"/>
-      <c r="S17" s="21"/>
-      <c r="T17" s="21"/>
-      <c r="U17" s="21"/>
-      <c r="V17" s="21"/>
-      <c r="W17" s="21"/>
-      <c r="X17" s="21"/>
-      <c r="Y17" s="21"/>
-      <c r="Z17" s="21"/>
-      <c r="AA17" s="21"/>
-      <c r="AB17" s="21"/>
-      <c r="AC17" s="21"/>
-      <c r="AD17" s="21"/>
-      <c r="AE17" s="21"/>
-      <c r="AF17" s="21"/>
-      <c r="AG17" s="22"/>
-      <c r="AH17" s="23">
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="20"/>
+      <c r="T17" s="20"/>
+      <c r="U17" s="20"/>
+      <c r="V17" s="20"/>
+      <c r="W17" s="20"/>
+      <c r="X17" s="20"/>
+      <c r="Y17" s="20"/>
+      <c r="Z17" s="20"/>
+      <c r="AA17" s="20"/>
+      <c r="AB17" s="20"/>
+      <c r="AC17" s="20"/>
+      <c r="AD17" s="20"/>
+      <c r="AE17" s="20"/>
+      <c r="AF17" s="20"/>
+      <c r="AG17" s="21"/>
+      <c r="AH17" s="22">
         <f>SUM(C17:AG17)</f>
         <v>0</v>
       </c>
-      <c r="AI17" s="24">
+      <c r="AI17" s="23">
         <f>COUNT(C17:AG17)</f>
         <v>0</v>
       </c>
-      <c r="AJ17" s="25">
+      <c r="AJ17" s="24">
         <f>AH18</f>
         <v>0</v>
       </c>
@@ -2354,134 +2732,134 @@
         <v/>
       </c>
       <c r="D18" s="11" t="str">
-        <f t="shared" ref="D18:AG18" si="10">IF(D17-8&gt;0,D17-8," ")</f>
+        <f t="shared" ref="D18:AG18" si="7">IF(D17-8&gt;0,D17-8," ")</f>
         <v/>
       </c>
       <c r="E18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="G18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="J18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="M18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="O18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="P18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Q18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="R18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="S18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="T18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="U18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="V18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="W18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="X18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Y18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Z18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AA18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AB18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AC18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AD18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AE18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AF18" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AG18" s="11" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="AH18" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AH18" s="14">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI18" s="4">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AJ18" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="15">
         <f>AH17+AH18</f>
         <v>0</v>
       </c>
@@ -2496,52 +2874,46 @@
   </mergeCells>
   <phoneticPr fontId="3"/>
   <conditionalFormatting sqref="B2:C2 J2:AJ2">
-    <cfRule type="containsText" dxfId="13" priority="23" operator="containsText" text="休">
-      <formula>NOT(ISERROR(SEARCH("休",B2)))</formula>
+    <cfRule type="containsText" dxfId="23" priority="24" operator="containsText" text="振">
+      <formula>NOT(ISERROR(SEARCH("振",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="22" operator="containsText" text="欠">
+    <cfRule type="containsText" dxfId="22" priority="25" operator="containsText" text="欠">
       <formula>NOT(ISERROR(SEARCH("欠",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="21" operator="containsText" text="振">
-      <formula>NOT(ISERROR(SEARCH("振",B2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:AJ18">
-    <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="振">
-      <formula>NOT(ISERROR(SEARCH("振",B3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="欠">
-      <formula>NOT(ISERROR(SEARCH("欠",B3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="休">
-      <formula>NOT(ISERROR(SEARCH("休",B3)))</formula>
+    <cfRule type="containsText" dxfId="21" priority="26" operator="containsText" text="休">
+      <formula>NOT(ISERROR(SEARCH("休",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:AG6">
-    <cfRule type="cellIs" dxfId="7" priority="25" operator="equal">
-      <formula>"日"</formula>
+    <cfRule type="expression" dxfId="20" priority="3" stopIfTrue="1">
+      <formula>C$6="日"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="24" operator="containsText" text="土">
-      <formula>NOT(ISERROR(SEARCH("土",C6)))</formula>
+    <cfRule type="expression" dxfId="12" priority="1">
+      <formula>C$6="土"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:AG8">
-    <cfRule type="top10" dxfId="5" priority="26" percent="1" rank="100"/>
+    <cfRule type="top10" dxfId="19" priority="29" percent="1" rank="100"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:AG10">
-    <cfRule type="top10" dxfId="4" priority="20" percent="1" rank="100"/>
+    <cfRule type="top10" dxfId="18" priority="23" percent="1" rank="100"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:AG12">
-    <cfRule type="top10" dxfId="3" priority="16" percent="1" rank="100"/>
+    <cfRule type="top10" dxfId="17" priority="19" percent="1" rank="100"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:AG14">
-    <cfRule type="top10" dxfId="2" priority="12" percent="1" rank="100"/>
+    <cfRule type="top10" dxfId="16" priority="15" percent="1" rank="100"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:AG16">
-    <cfRule type="top10" dxfId="1" priority="8" percent="1" rank="100"/>
+    <cfRule type="top10" dxfId="15" priority="11" percent="1" rank="100"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:AG18">
-    <cfRule type="top10" dxfId="0" priority="4" percent="1" rank="100"/>
+    <cfRule type="top10" dxfId="14" priority="7" percent="1" rank="100"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA6">
+    <cfRule type="expression" dxfId="13" priority="2">
+      <formula>C$6="日"</formula>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>